<commit_message>
Matches services, first tests
</commit_message>
<xml_diff>
--- a/process/Hours.xlsx
+++ b/process/Hours.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\mofiler\WorldCup\process\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\worldcup\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -478,7 +478,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -526,7 +526,7 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <f>SUM(B5:B12)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More match services with tests; list matches first page; matches.json loaded at startup
</commit_message>
<xml_diff>
--- a/process/Hours.xlsx
+++ b/process/Hours.xlsx
@@ -458,7 +458,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +478,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -526,7 +526,7 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <f>SUM(B5:B12)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Read feed; update process
</commit_message>
<xml_diff>
--- a/process/Hours.xlsx
+++ b/process/Hours.xlsx
@@ -458,7 +458,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,24 +517,30 @@
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <f>SUM(B5:B12)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove match in views
</commit_message>
<xml_diff>
--- a/process/Hours.xlsx
+++ b/process/Hours.xlsx
@@ -134,7 +134,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -143,7 +143,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Énfasis3" xfId="2" builtinId="38"/>
@@ -452,7 +451,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -532,17 +531,17 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" s="4">
         <f>SUM(B5:B13)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Apply feed, with test
</commit_message>
<xml_diff>
--- a/process/Hours.xlsx
+++ b/process/Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Hours by Iteration</t>
   </si>
@@ -448,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -539,9 +539,17 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="B14" s="4">
-        <f>SUM(B5:B13)</f>
-        <v>16</v>
+      <c r="A14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="B15" s="4">
+        <f>SUM(B5:B14)</f>
+        <v>16.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New API file, updated status
</commit_message>
<xml_diff>
--- a/process/Hours.xlsx
+++ b/process/Hours.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Hours by Iteration</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>#2</t>
+  </si>
+  <si>
+    <t>#3</t>
   </si>
 </sst>
 </file>
@@ -458,28 +461,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C14"/>
+      <selection activeCell="D6" sqref="D6:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -487,8 +493,11 @@
         <v>2</v>
       </c>
       <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -496,8 +505,9 @@
         <v>3</v>
       </c>
       <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -505,8 +515,9 @@
         <v>2</v>
       </c>
       <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -514,8 +525,9 @@
         <v>2</v>
       </c>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -525,8 +537,9 @@
       <c r="C9" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -534,8 +547,9 @@
         <v>2</v>
       </c>
       <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -543,8 +557,9 @@
         <v>0</v>
       </c>
       <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>2</v>
       </c>
@@ -552,8 +567,9 @@
         <v>1</v>
       </c>
       <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
@@ -561,8 +577,9 @@
         <v>3</v>
       </c>
       <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
@@ -570,8 +587,9 @@
         <v>2</v>
       </c>
       <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <f>SUM(B5:B14)</f>
         <v>18</v>
@@ -579,6 +597,10 @@
       <c r="C15" s="5">
         <f>SUM(C5:C14)</f>
         <v>2</v>
+      </c>
+      <c r="D15" s="5">
+        <f>SUM(D5:D14)</f>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Additional control in feed, process updated
</commit_message>
<xml_diff>
--- a/process/Hours.xlsx
+++ b/process/Hours.xlsx
@@ -460,7 +460,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -547,7 +547,9 @@
       <c r="D9" s="1">
         <v>0.5</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
@@ -625,7 +627,7 @@
       </c>
       <c r="E15" s="5">
         <f>SUM(E5:E14)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new field to views, fixing width field
</commit_message>
<xml_diff>
--- a/process/Hours.xlsx
+++ b/process/Hours.xlsx
@@ -470,7 +470,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +610,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -660,7 +660,7 @@
       </c>
       <c r="F15" s="5">
         <f>SUM(F5:F14)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>